<commit_message>
updated w ens results
</commit_message>
<xml_diff>
--- a/07_documents/modeling_results.xlsx
+++ b/07_documents/modeling_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanwegner/Desktop/nba2/07_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BE3FB8-68D4-9E40-945C-E11AE45FA91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2699B3C8-3860-9C48-9E54-1EB5C9C7EE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{DEEB7051-5BA9-3245-9906-EC424B1E6021}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Modeling Results </t>
   </si>
@@ -60,13 +60,41 @@
   </si>
   <si>
     <t>Test Drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensemble - All </t>
+  </si>
+  <si>
+    <t>Ensemble - LinReg and PCR</t>
+  </si>
+  <si>
+    <t>Ensemble - LinReg and EN</t>
+  </si>
+  <si>
+    <t>Ensemble - LinReg and LGBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - I'm selecting this one because of the stability and train performance </t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Gain vs Baseline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,16 +109,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -98,20 +140,171 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -421,94 +614,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EF62A4-C9A3-7A48-90C7-8F60AA47FD84}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="F3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3.65200045588655</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>3.5018859134870599</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <f>(D4-C4)/C4</f>
         <v>-4.1104743609088258E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="F4" s="4">
+        <f>(C$4-C4)/C4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <f>(D$4-D4)/D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>3.6668997429448602</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>3.5917639484991799</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <f>(D5-C5)/C5</f>
         <v>-2.0490277813087765E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:G11" si="0">(C$4-C5)/C5</f>
+        <v>-4.0631836436151704E-3</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.502336910243658E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5.1956905219614402</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>4.6619023298792204</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <f>(D6-C6)/C6</f>
         <v>-0.10273671802159377</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.29710970265644832</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.24882898317224375</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>3.6939736427288801</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>3.62571676752387</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <f>(D7-C7)/C7</f>
         <v>-1.8477899900386442E-2</v>
       </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.1362611350773712E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.4153482463380201E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.55770720394914</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.5211100756339602</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" ref="E8:E11" si="1">(D8-C8)/C8</f>
+        <v>-1.028671732023257E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6503938219745077E-2</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.4596879205598345E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.6514813818485301</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.5081757577497399</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>-3.9245886562960651E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.421543707165492E-4</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.792910246524961E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3.65200045588655</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3.5018859134870701</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>-4.1104743609085462E-2</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>-2.916728893769301E-15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="10">
+        <v>3.5566426625019698</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3.5198011788479699</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>-1.0358500178391046E-2</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>2.6811181901951153E-2</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>-5.089851514503356E-3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:C11">
+    <cfRule type="top10" dxfId="1" priority="2" stopIfTrue="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D11">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ready for stage II
</commit_message>
<xml_diff>
--- a/07_documents/modeling_results.xlsx
+++ b/07_documents/modeling_results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanwegner/Desktop/nba2/07_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2699B3C8-3860-9C48-9E54-1EB5C9C7EE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A24DA5-97F2-4646-B72A-0C6BCDBE4179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{DEEB7051-5BA9-3245-9906-EC424B1E6021}"/>
+    <workbookView xWindow="-35380" yWindow="1240" windowWidth="24980" windowHeight="14520" xr2:uid="{DEEB7051-5BA9-3245-9906-EC424B1E6021}"/>
   </bookViews>
   <sheets>
-    <sheet name="2023_Preseason" sheetId="1" r:id="rId1"/>
+    <sheet name="2023" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t xml:space="preserve">Modeling Results </t>
   </si>
@@ -74,9 +74,6 @@
     <t>Ensemble - LinReg and LGBM</t>
   </si>
   <si>
-    <t xml:space="preserve"> - I'm selecting this one because of the stability and train performance </t>
-  </si>
-  <si>
     <t>Train</t>
   </si>
   <si>
@@ -84,6 +81,66 @@
   </si>
   <si>
     <t>Gain vs Baseline</t>
+  </si>
+  <si>
+    <t>Added last season playoff wins, conference rank, and an indicator for made the poffs</t>
+  </si>
+  <si>
+    <t>With Scaling</t>
+  </si>
+  <si>
+    <t>Final Candidate?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>with LGBM 2</t>
+  </si>
+  <si>
+    <t>With LGBM 1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Train: BC?</t>
+  </si>
+  <si>
+    <t>Cutoff</t>
+  </si>
+  <si>
+    <t>Test: BC?</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Next Stage</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need to reduce features somehow. More optimization is possible</t>
+  </si>
+  <si>
+    <t>As a component of Ensemble</t>
+  </si>
+  <si>
+    <t>ENS - LR, PCR, LGBM</t>
+  </si>
+  <si>
+    <t>ENS - LR, PCR</t>
+  </si>
+  <si>
+    <t>ENS - LR, LGBM</t>
+  </si>
+  <si>
+    <t>Stage I</t>
+  </si>
+  <si>
+    <t>Stage II</t>
   </si>
 </sst>
 </file>
@@ -91,12 +148,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,8 +181,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +210,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -169,16 +284,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -187,120 +331,125 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="3"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="3"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="3"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{B5F8CE8D-D526-43E0-B31D-295D9E2517C6}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -614,239 +763,847 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EF62A4-C9A3-7A48-90C7-8F60AA47FD84}">
-  <dimension ref="B2:H11"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="5" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="2:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="15" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4">
+        <v>3.55</v>
+      </c>
+      <c r="K4">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C6" s="2">
         <v>3.65200045588655</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D6" s="2">
         <v>3.5018859134870599</v>
       </c>
-      <c r="E4" s="3">
-        <f>(D4-C4)/C4</f>
+      <c r="E6" s="3">
+        <f>(D6-C6)/C6</f>
         <v>-4.1104743609088258E-2</v>
       </c>
-      <c r="F4" s="4">
-        <f>(C$4-C4)/C4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <f>(D$4-D4)/D4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="F6" s="4">
+        <f>(C$6-C6)/C6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <f>(D$6-D6)/D6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="26" t="b">
+        <f>C6&lt;$J$4</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="26" t="b">
+        <f>D6&lt;$K$4</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="27"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C7" s="2">
         <v>3.6668997429448602</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D7" s="2">
         <v>3.5917639484991799</v>
       </c>
-      <c r="E5" s="3">
-        <f>(D5-C5)/C5</f>
+      <c r="E7" s="3">
+        <f>(D7-C7)/C7</f>
         <v>-2.0490277813087765E-2</v>
       </c>
-      <c r="F5" s="4">
-        <f t="shared" ref="F5:G11" si="0">(C$4-C5)/C5</f>
+      <c r="F7" s="4">
+        <f t="shared" ref="F7:G13" si="0">(C$6-C7)/C7</f>
         <v>-4.0631836436151704E-3</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>-2.502336910243658E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="H7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="26" t="b">
+        <f t="shared" ref="J7:J25" si="1">C7&lt;$J$4</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="26" t="b">
+        <f t="shared" ref="K7:K25" si="2">D7&lt;$K$4</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="N7" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
         <v>5.1956905219614402</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="2">
         <v>4.6619023298792204</v>
       </c>
-      <c r="E6" s="3">
-        <f>(D6-C6)/C6</f>
+      <c r="E8" s="3">
+        <f>(D8-C8)/C8</f>
         <v>-0.10273671802159377</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>-0.29710970265644832</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>-0.24882898317224375</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+      <c r="H8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="N8" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
         <v>3.6939736427288801</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="2">
         <v>3.62571676752387</v>
       </c>
-      <c r="E7" s="3">
-        <f>(D7-C7)/C7</f>
+      <c r="E9" s="3">
+        <f>(D9-C9)/C9</f>
         <v>-1.8477899900386442E-2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>-1.1362611350773712E-2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>-3.4153482463380201E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="H9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="27"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C10" s="2">
         <v>3.55770720394914</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D10" s="2">
         <v>3.5211100756339602</v>
       </c>
-      <c r="E8" s="3">
-        <f t="shared" ref="E8:E11" si="1">(D8-C8)/C8</f>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E13" si="3">(D10-C10)/C10</f>
         <v>-1.028671732023257E-2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>2.6503938219745077E-2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>-5.4596879205598345E-3</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="H10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="2">
         <v>3.6514813818485301</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D11" s="2">
         <v>3.5081757577497399</v>
       </c>
-      <c r="E9" s="3">
-        <f t="shared" si="1"/>
+      <c r="E11" s="3">
+        <f t="shared" si="3"/>
         <v>-3.9245886562960651E-2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>1.421543707165492E-4</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>-1.792910246524961E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="H11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="27"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C12" s="5">
         <v>3.65200045588655</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D12" s="5">
         <v>3.5018859134870701</v>
       </c>
-      <c r="E10" s="7">
-        <f t="shared" si="1"/>
+      <c r="E12" s="6">
+        <f t="shared" si="3"/>
         <v>-4.1104743609085462E-2</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>-2.916728893769301E-15</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="H12" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C13" s="2">
         <v>3.5566426625019698</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D13" s="2">
         <v>3.5198011788479699</v>
       </c>
-      <c r="E11" s="11">
-        <f t="shared" si="1"/>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
         <v>-1.0358500178391046E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>2.6811181901951153E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>-5.089851514503356E-3</v>
       </c>
-      <c r="H11" t="s">
-        <v>12</v>
+      <c r="H13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3.5924</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3.4134980000000001</v>
+      </c>
+      <c r="E14" s="11">
+        <f>(D14-C14)/C14</f>
+        <v>-4.9800133615410282E-2</v>
+      </c>
+      <c r="F14" s="12">
+        <f>(C$6-C14)/C14</f>
+        <v>1.6590707016632317E-2</v>
+      </c>
+      <c r="G14" s="12">
+        <f>(D$6-D14)/D14</f>
+        <v>2.5893647363220883E-2</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3.603634</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3.4792209999999999</v>
+      </c>
+      <c r="E15" s="3">
+        <f>(D15-C15)/C15</f>
+        <v>-3.4524316287392144E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" ref="F15:G23" si="4">(C$6-C15)/C15</f>
+        <v>1.3421578297504679E-2</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="4"/>
+        <v>6.5143644186615376E-3</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5.1615500000000001</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4.9933290000000001</v>
+      </c>
+      <c r="E16" s="3">
+        <f>(D16-C16)/C16</f>
+        <v>-3.2591179006306238E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.29246050975258403</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.29868712566565114</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.6174759999999999</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.4967890000000001</v>
+      </c>
+      <c r="E17" s="3">
+        <f>(D17-C17)/C17</f>
+        <v>-3.336221166360185E-2</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="4"/>
+        <v>9.5437968037797808E-3</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="4"/>
+        <v>1.4575982385725194E-3</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.5473710000000001</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.4695369999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" ref="E18:E23" si="5">(D18-C18)/C18</f>
+        <v>-2.1941319360168469E-2</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="4"/>
+        <v>2.9494929029568635E-2</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="4"/>
+        <v>9.3236975098003102E-3</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="24" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.4985729999999999</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3.4403739999999998</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" ref="E19" si="6">(D19-C19)/C19</f>
+        <v>-1.6635068069181382E-2</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" ref="F19" si="7">(C$6-C19)/C19</f>
+        <v>4.3854295990551018E-2</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" ref="G19" si="8">(D$6-D19)/D19</f>
+        <v>1.7879426331863946E-2</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="25" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.5921829999999999</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3.4172709999999999</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="5"/>
+        <v>-4.8692396796042953E-2</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="4"/>
+        <v>1.6652118192906674E-2</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="4"/>
+        <v>2.4760960862354773E-2</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3.5924</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3.4134980000000001</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="5"/>
+        <v>-4.9800133615410282E-2</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6590707016632317E-2</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="4"/>
+        <v>2.5893647363220883E-2</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.5497519999999998</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.4762960000000001</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" ref="E22" si="9">(D22-C22)/C22</f>
+        <v>-2.0693276600731472E-2</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" ref="F22" si="10">(C$6-C22)/C22</f>
+        <v>2.8804394190509699E-2</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" ref="G22" si="11">(D$6-D22)/D22</f>
+        <v>7.3612585024577471E-3</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="24" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.503352</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.4479980000000001</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="5"/>
+        <v>-1.5800296401845975E-2</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="4"/>
+        <v>4.2430351242624197E-2</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="4"/>
+        <v>1.5628754276266921E-2</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="25" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.6432630000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.5646429999999998</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" ref="E24:E25" si="12">(D24-C24)/C24</f>
+        <v>-2.1579556567835029E-2</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" ref="F24:F25" si="13">(C$6-C24)/C24</f>
+        <v>2.3982501089133117E-3</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" ref="G24:G25" si="14">(D$6-D24)/D24</f>
+        <v>-1.760543384370886E-2</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5.4501379999999999</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5.151052</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="12"/>
+        <v>-5.4876775597241752E-2</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="13"/>
+        <v>-0.32992514026497127</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="14"/>
+        <v>-0.32016102468251922</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="B28" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="3">
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:C11">
-    <cfRule type="top10" dxfId="1" priority="2" stopIfTrue="1" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="C6:C25">
+    <cfRule type="top10" dxfId="3" priority="4" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D11">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="D6:D25">
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H25">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",H6)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>